<commit_message>
se prueba y adabta el bot que descarga los soportes de wormanager al flujo dos, falta es corregir diccionario global y adecuar plantilla de reporte para reportar eventos en siesa 8.5
</commit_message>
<xml_diff>
--- a/Input/Archivo de Seguimiento.xlsx
+++ b/Input/Archivo de Seguimiento.xlsx
@@ -18382,17 +18382,17 @@
       </c>
       <c r="H446" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No descargado</t>
         </is>
       </c>
       <c r="I446" t="inlineStr">
         <is>
-          <t>30-10-2025 06:07:17</t>
+          <t>31-10-2025 20:04:21</t>
         </is>
       </c>
       <c r="J446" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>No se encontraron resultados de la busqueda. Chequear manualmente el nombre correcto a buscar.</t>
         </is>
       </c>
     </row>
@@ -18782,17 +18782,17 @@
       </c>
       <c r="H456" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No descargado</t>
         </is>
       </c>
       <c r="I456" t="inlineStr">
         <is>
-          <t>30-10-2025 06:08:57</t>
+          <t>03-11-2025 07:35:39</t>
         </is>
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>No se encontraron resultados de la busqueda. Chequear manualmente el nombre correcto a buscar.</t>
         </is>
       </c>
     </row>
@@ -19140,19 +19140,19 @@
           <t>PE-223</t>
         </is>
       </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>13980</t>
+        </is>
+      </c>
       <c r="H465" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Procesado</t>
         </is>
       </c>
       <c r="I465" t="inlineStr">
         <is>
-          <t>30-10-2025 06:10:38</t>
-        </is>
-      </c>
-      <c r="J465" t="inlineStr">
-        <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>03-11-2025 08:03:32</t>
         </is>
       </c>
     </row>
@@ -20022,17 +20022,17 @@
       </c>
       <c r="H487" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No descargado</t>
         </is>
       </c>
       <c r="I487" t="inlineStr">
         <is>
-          <t>30-10-2025 06:12:18</t>
+          <t>03-11-2025 08:05:06</t>
         </is>
       </c>
       <c r="J487" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>No se encontraron resultados de la busqueda. Chequear manualmente el nombre correcto a buscar.</t>
         </is>
       </c>
     </row>
@@ -20342,17 +20342,17 @@
       </c>
       <c r="H495" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No descargado</t>
         </is>
       </c>
       <c r="I495" t="inlineStr">
         <is>
-          <t>30-10-2025 06:13:58</t>
+          <t>03-11-2025 08:06:41</t>
         </is>
       </c>
       <c r="J495" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>No se encontraron resultados de la busqueda. Chequear manualmente el nombre correcto a buscar.</t>
         </is>
       </c>
     </row>
@@ -20662,17 +20662,17 @@
       </c>
       <c r="H503" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No descargado</t>
         </is>
       </c>
       <c r="I503" t="inlineStr">
         <is>
-          <t>30-10-2025 06:15:39</t>
+          <t>03-11-2025 08:08:16</t>
         </is>
       </c>
       <c r="J503" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>No se encontraron resultados de la busqueda. Chequear manualmente el nombre correcto a buscar.</t>
         </is>
       </c>
     </row>
@@ -21462,17 +21462,17 @@
       </c>
       <c r="H523" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No descargado</t>
         </is>
       </c>
       <c r="I523" t="inlineStr">
         <is>
-          <t>30-10-2025 06:17:20</t>
+          <t>03-11-2025 08:09:52</t>
         </is>
       </c>
       <c r="J523" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>No se encontraron resultados de la busqueda. Chequear manualmente el nombre correcto a buscar.</t>
         </is>
       </c>
     </row>
@@ -21712,12 +21712,12 @@
       </c>
       <c r="I529" t="inlineStr">
         <is>
-          <t>30-10-2025 06:19:00</t>
+          <t>03-11-2025 10:53:13</t>
         </is>
       </c>
       <c r="J529" t="inlineStr">
         <is>
-          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -21757,7 +21757,7 @@
       </c>
       <c r="I530" t="inlineStr">
         <is>
-          <t>30-10-2025 06:35:25</t>
+          <t>03-11-2025 11:09:13</t>
         </is>
       </c>
       <c r="J530" t="inlineStr">
@@ -21802,7 +21802,7 @@
       </c>
       <c r="I531" t="inlineStr">
         <is>
-          <t>30-10-2025 06:51:32</t>
+          <t>03-11-2025 11:25:06</t>
         </is>
       </c>
       <c r="J531" t="inlineStr">
@@ -21847,7 +21847,7 @@
       </c>
       <c r="I532" t="inlineStr">
         <is>
-          <t>30-10-2025 07:07:39</t>
+          <t>03-11-2025 11:40:59</t>
         </is>
       </c>
       <c r="J532" t="inlineStr">
@@ -21892,7 +21892,7 @@
       </c>
       <c r="I533" t="inlineStr">
         <is>
-          <t>30-10-2025 07:23:46</t>
+          <t>03-11-2025 11:56:52</t>
         </is>
       </c>
       <c r="J533" t="inlineStr">
@@ -21937,7 +21937,7 @@
       </c>
       <c r="I534" t="inlineStr">
         <is>
-          <t>30-10-2025 07:39:54</t>
+          <t>03-11-2025 12:12:45</t>
         </is>
       </c>
       <c r="J534" t="inlineStr">
@@ -21982,7 +21982,7 @@
       </c>
       <c r="I535" t="inlineStr">
         <is>
-          <t>30-10-2025 07:55:56</t>
+          <t>03-11-2025 12:28:38</t>
         </is>
       </c>
       <c r="J535" t="inlineStr">
@@ -22027,7 +22027,7 @@
       </c>
       <c r="I536" t="inlineStr">
         <is>
-          <t>30-10-2025 08:12:05</t>
+          <t>03-11-2025 12:44:32</t>
         </is>
       </c>
       <c r="J536" t="inlineStr">
@@ -22072,7 +22072,7 @@
       </c>
       <c r="I537" t="inlineStr">
         <is>
-          <t>30-10-2025 08:28:14</t>
+          <t>03-11-2025 13:00:26</t>
         </is>
       </c>
       <c r="J537" t="inlineStr">
@@ -22117,7 +22117,7 @@
       </c>
       <c r="I538" t="inlineStr">
         <is>
-          <t>30-10-2025 08:44:24</t>
+          <t>03-11-2025 13:16:21</t>
         </is>
       </c>
       <c r="J538" t="inlineStr">
@@ -22162,7 +22162,7 @@
       </c>
       <c r="I539" t="inlineStr">
         <is>
-          <t>30-10-2025 09:00:33</t>
+          <t>03-11-2025 13:32:16</t>
         </is>
       </c>
       <c r="J539" t="inlineStr">
@@ -22207,7 +22207,7 @@
       </c>
       <c r="I540" t="inlineStr">
         <is>
-          <t>30-10-2025 09:16:42</t>
+          <t>03-11-2025 13:48:11</t>
         </is>
       </c>
       <c r="J540" t="inlineStr">
@@ -22252,7 +22252,7 @@
       </c>
       <c r="I541" t="inlineStr">
         <is>
-          <t>30-10-2025 09:32:52</t>
+          <t>03-11-2025 14:04:06</t>
         </is>
       </c>
       <c r="J541" t="inlineStr">
@@ -22297,7 +22297,7 @@
       </c>
       <c r="I542" t="inlineStr">
         <is>
-          <t>30-10-2025 09:49:01</t>
+          <t>03-11-2025 14:20:01</t>
         </is>
       </c>
       <c r="J542" t="inlineStr">
@@ -22342,7 +22342,7 @@
       </c>
       <c r="I543" t="inlineStr">
         <is>
-          <t>30-10-2025 10:04:52</t>
+          <t>03-11-2025 14:35:57</t>
         </is>
       </c>
       <c r="J543" t="inlineStr">
@@ -22387,7 +22387,7 @@
       </c>
       <c r="I544" t="inlineStr">
         <is>
-          <t>30-10-2025 10:21:22</t>
+          <t>03-11-2025 14:51:52</t>
         </is>
       </c>
       <c r="J544" t="inlineStr">
@@ -22432,7 +22432,7 @@
       </c>
       <c r="I545" t="inlineStr">
         <is>
-          <t>30-10-2025 10:37:33</t>
+          <t>03-11-2025 15:07:50</t>
         </is>
       </c>
       <c r="J545" t="inlineStr">
@@ -22477,7 +22477,7 @@
       </c>
       <c r="I546" t="inlineStr">
         <is>
-          <t>30-10-2025 10:53:24</t>
+          <t>03-11-2025 15:23:46</t>
         </is>
       </c>
       <c r="J546" t="inlineStr">
@@ -22522,7 +22522,7 @@
       </c>
       <c r="I547" t="inlineStr">
         <is>
-          <t>30-10-2025 11:09:16</t>
+          <t>03-11-2025 15:39:42</t>
         </is>
       </c>
       <c r="J547" t="inlineStr">
@@ -22567,7 +22567,7 @@
       </c>
       <c r="I548" t="inlineStr">
         <is>
-          <t>30-10-2025 11:25:08</t>
+          <t>03-11-2025 15:55:39</t>
         </is>
       </c>
       <c r="J548" t="inlineStr">
@@ -22612,7 +22612,7 @@
       </c>
       <c r="I549" t="inlineStr">
         <is>
-          <t>30-10-2025 11:41:18</t>
+          <t>03-11-2025 16:11:36</t>
         </is>
       </c>
       <c r="J549" t="inlineStr">
@@ -22657,7 +22657,7 @@
       </c>
       <c r="I550" t="inlineStr">
         <is>
-          <t>30-10-2025 11:57:11</t>
+          <t>03-11-2025 16:27:34</t>
         </is>
       </c>
       <c r="J550" t="inlineStr">
@@ -22702,7 +22702,7 @@
       </c>
       <c r="I551" t="inlineStr">
         <is>
-          <t>30-10-2025 12:13:05</t>
+          <t>03-11-2025 16:43:32</t>
         </is>
       </c>
       <c r="J551" t="inlineStr">
@@ -22747,7 +22747,7 @@
       </c>
       <c r="I552" t="inlineStr">
         <is>
-          <t>30-10-2025 12:26:42</t>
+          <t>03-11-2025 16:59:30</t>
         </is>
       </c>
       <c r="J552" t="inlineStr">
@@ -22792,7 +22792,7 @@
       </c>
       <c r="I553" t="inlineStr">
         <is>
-          <t>29-10-2025 21:07:48</t>
+          <t>03-11-2025 17:15:28</t>
         </is>
       </c>
       <c r="J553" t="inlineStr">
@@ -22837,7 +22837,7 @@
       </c>
       <c r="I554" t="inlineStr">
         <is>
-          <t>29-10-2025 21:23:46</t>
+          <t>03-11-2025 17:31:27</t>
         </is>
       </c>
       <c r="J554" t="inlineStr">
@@ -22882,12 +22882,12 @@
       </c>
       <c r="I555" t="inlineStr">
         <is>
-          <t>29-10-2025 21:39:43</t>
+          <t>03-11-2025 09:04:33</t>
         </is>
       </c>
       <c r="J555" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -22927,12 +22927,12 @@
       </c>
       <c r="I556" t="inlineStr">
         <is>
-          <t>29-10-2025 21:55:40</t>
+          <t>03-11-2025 09:04:43</t>
         </is>
       </c>
       <c r="J556" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -22972,12 +22972,12 @@
       </c>
       <c r="I557" t="inlineStr">
         <is>
-          <t>29-10-2025 22:11:38</t>
+          <t>03-11-2025 09:04:50</t>
         </is>
       </c>
       <c r="J557" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23017,12 +23017,12 @@
       </c>
       <c r="I558" t="inlineStr">
         <is>
-          <t>29-10-2025 22:27:36</t>
+          <t>03-11-2025 09:04:58</t>
         </is>
       </c>
       <c r="J558" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23062,12 +23062,12 @@
       </c>
       <c r="I559" t="inlineStr">
         <is>
-          <t>29-10-2025 22:43:34</t>
+          <t>03-11-2025 09:05:05</t>
         </is>
       </c>
       <c r="J559" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23107,12 +23107,12 @@
       </c>
       <c r="I560" t="inlineStr">
         <is>
-          <t>29-10-2025 22:59:33</t>
+          <t>03-11-2025 09:05:13</t>
         </is>
       </c>
       <c r="J560" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23152,12 +23152,12 @@
       </c>
       <c r="I561" t="inlineStr">
         <is>
-          <t>29-10-2025 23:15:32</t>
+          <t>03-11-2025 09:05:21</t>
         </is>
       </c>
       <c r="J561" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23197,12 +23197,12 @@
       </c>
       <c r="I562" t="inlineStr">
         <is>
-          <t>29-10-2025 23:31:31</t>
+          <t>03-11-2025 07:05:27</t>
         </is>
       </c>
       <c r="J562" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23242,12 +23242,12 @@
       </c>
       <c r="I563" t="inlineStr">
         <is>
-          <t>29-10-2025 23:47:49</t>
+          <t>03-11-2025 07:05:34</t>
         </is>
       </c>
       <c r="J563" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23287,12 +23287,12 @@
       </c>
       <c r="I564" t="inlineStr">
         <is>
-          <t>30-10-2025 00:03:49</t>
+          <t>03-11-2025 07:05:41</t>
         </is>
       </c>
       <c r="J564" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23332,12 +23332,12 @@
       </c>
       <c r="I565" t="inlineStr">
         <is>
-          <t>30-10-2025 00:19:49</t>
+          <t>03-11-2025 07:05:49</t>
         </is>
       </c>
       <c r="J565" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23377,12 +23377,12 @@
       </c>
       <c r="I566" t="inlineStr">
         <is>
-          <t>30-10-2025 00:35:48</t>
+          <t>03-11-2025 07:05:56</t>
         </is>
       </c>
       <c r="J566" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23422,12 +23422,12 @@
       </c>
       <c r="I567" t="inlineStr">
         <is>
-          <t>30-10-2025 00:51:48</t>
+          <t>03-11-2025 07:06:03</t>
         </is>
       </c>
       <c r="J567" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23467,12 +23467,12 @@
       </c>
       <c r="I568" t="inlineStr">
         <is>
-          <t>30-10-2025 01:07:48</t>
+          <t>03-11-2025 07:06:11</t>
         </is>
       </c>
       <c r="J568" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23512,12 +23512,12 @@
       </c>
       <c r="I569" t="inlineStr">
         <is>
-          <t>30-10-2025 01:23:49</t>
+          <t>03-11-2025 07:06:19</t>
         </is>
       </c>
       <c r="J569" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -23557,12 +23557,12 @@
       </c>
       <c r="I570" t="inlineStr">
         <is>
-          <t>30-10-2025 01:39:50</t>
+          <t>03-11-2025 07:06:26</t>
         </is>
       </c>
       <c r="J570" t="inlineStr">
         <is>
-          <t>Ocurrio un error al descargar documentos de Workmanager. Revisar archivo de logs.</t>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>
@@ -25277,7 +25277,7 @@
       </c>
       <c r="I613" t="inlineStr">
         <is>
-          <t>30-10-2025 03:43:50</t>
+          <t>03-11-2025 07:06:34</t>
         </is>
       </c>
       <c r="J613" t="inlineStr">
@@ -25357,7 +25357,7 @@
       </c>
       <c r="I615" t="inlineStr">
         <is>
-          <t>30-10-2025 03:45:35</t>
+          <t>03-11-2025 07:06:42</t>
         </is>
       </c>
       <c r="J615" t="inlineStr">
@@ -25517,7 +25517,7 @@
       </c>
       <c r="I619" t="inlineStr">
         <is>
-          <t>30-10-2025 03:55:23</t>
+          <t>03-11-2025 07:06:49</t>
         </is>
       </c>
       <c r="J619" t="inlineStr">
@@ -25597,7 +25597,7 @@
       </c>
       <c r="I621" t="inlineStr">
         <is>
-          <t>30-10-2025 03:57:09</t>
+          <t>03-11-2025 07:06:56</t>
         </is>
       </c>
       <c r="J621" t="inlineStr">
@@ -25677,7 +25677,7 @@
       </c>
       <c r="I623" t="inlineStr">
         <is>
-          <t>30-10-2025 03:58:54</t>
+          <t>03-11-2025 07:07:04</t>
         </is>
       </c>
       <c r="J623" t="inlineStr">
@@ -25917,7 +25917,7 @@
       </c>
       <c r="I629" t="inlineStr">
         <is>
-          <t>30-10-2025 04:13:45</t>
+          <t>03-11-2025 07:07:12</t>
         </is>
       </c>
       <c r="J629" t="inlineStr">
@@ -25997,7 +25997,7 @@
       </c>
       <c r="I631" t="inlineStr">
         <is>
-          <t>30-10-2025 04:15:32</t>
+          <t>03-11-2025 07:07:19</t>
         </is>
       </c>
       <c r="J631" t="inlineStr">
@@ -26077,7 +26077,7 @@
       </c>
       <c r="I633" t="inlineStr">
         <is>
-          <t>30-10-2025 04:17:18</t>
+          <t>03-11-2025 07:07:27</t>
         </is>
       </c>
       <c r="J633" t="inlineStr">
@@ -26157,7 +26157,7 @@
       </c>
       <c r="I635" t="inlineStr">
         <is>
-          <t>30-10-2025 04:19:04</t>
+          <t>03-11-2025 07:07:35</t>
         </is>
       </c>
       <c r="J635" t="inlineStr">
@@ -26237,7 +26237,7 @@
       </c>
       <c r="I637" t="inlineStr">
         <is>
-          <t>30-10-2025 04:20:51</t>
+          <t>03-11-2025 07:07:42</t>
         </is>
       </c>
       <c r="J637" t="inlineStr">
@@ -26317,7 +26317,7 @@
       </c>
       <c r="I639" t="inlineStr">
         <is>
-          <t>30-10-2025 04:22:36</t>
+          <t>03-11-2025 07:07:49</t>
         </is>
       </c>
       <c r="J639" t="inlineStr">
@@ -26397,7 +26397,7 @@
       </c>
       <c r="I641" t="inlineStr">
         <is>
-          <t>30-10-2025 04:24:23</t>
+          <t>03-11-2025 07:07:57</t>
         </is>
       </c>
       <c r="J641" t="inlineStr">
@@ -26477,7 +26477,7 @@
       </c>
       <c r="I643" t="inlineStr">
         <is>
-          <t>30-10-2025 04:26:10</t>
+          <t>03-11-2025 07:08:04</t>
         </is>
       </c>
       <c r="J643" t="inlineStr">
@@ -26557,7 +26557,7 @@
       </c>
       <c r="I645" t="inlineStr">
         <is>
-          <t>30-10-2025 04:27:57</t>
+          <t>03-11-2025 07:08:12</t>
         </is>
       </c>
       <c r="J645" t="inlineStr">
@@ -26637,7 +26637,7 @@
       </c>
       <c r="I647" t="inlineStr">
         <is>
-          <t>30-10-2025 04:29:43</t>
+          <t>03-11-2025 07:08:19</t>
         </is>
       </c>
       <c r="J647" t="inlineStr">
@@ -26717,7 +26717,7 @@
       </c>
       <c r="I649" t="inlineStr">
         <is>
-          <t>30-10-2025 04:31:30</t>
+          <t>03-11-2025 07:08:26</t>
         </is>
       </c>
       <c r="J649" t="inlineStr">
@@ -26797,7 +26797,7 @@
       </c>
       <c r="I651" t="inlineStr">
         <is>
-          <t>30-10-2025 04:33:16</t>
+          <t>03-11-2025 07:08:34</t>
         </is>
       </c>
       <c r="J651" t="inlineStr">
@@ -26877,7 +26877,7 @@
       </c>
       <c r="I653" t="inlineStr">
         <is>
-          <t>30-10-2025 04:35:02</t>
+          <t>03-11-2025 07:08:41</t>
         </is>
       </c>
       <c r="J653" t="inlineStr">
@@ -27077,7 +27077,7 @@
       </c>
       <c r="I658" t="inlineStr">
         <is>
-          <t>30-10-2025 04:49:13</t>
+          <t>03-11-2025 07:08:49</t>
         </is>
       </c>
       <c r="J658" t="inlineStr">
@@ -27197,7 +27197,7 @@
       </c>
       <c r="I661" t="inlineStr">
         <is>
-          <t>30-10-2025 04:55:48</t>
+          <t>03-11-2025 07:08:57</t>
         </is>
       </c>
       <c r="J661" t="inlineStr">
@@ -27277,7 +27277,7 @@
       </c>
       <c r="I663" t="inlineStr">
         <is>
-          <t>30-10-2025 04:57:34</t>
+          <t>03-11-2025 07:09:08</t>
         </is>
       </c>
       <c r="J663" t="inlineStr">
@@ -27357,7 +27357,7 @@
       </c>
       <c r="I665" t="inlineStr">
         <is>
-          <t>30-10-2025 04:59:20</t>
+          <t>03-11-2025 06:09:14</t>
         </is>
       </c>
       <c r="J665" t="inlineStr">
@@ -27437,7 +27437,7 @@
       </c>
       <c r="I667" t="inlineStr">
         <is>
-          <t>30-10-2025 05:01:06</t>
+          <t>03-11-2025 06:09:22</t>
         </is>
       </c>
       <c r="J667" t="inlineStr">
@@ -27517,7 +27517,7 @@
       </c>
       <c r="I669" t="inlineStr">
         <is>
-          <t>30-10-2025 05:02:53</t>
+          <t>03-11-2025 06:09:29</t>
         </is>
       </c>
       <c r="J669" t="inlineStr">
@@ -27597,7 +27597,7 @@
       </c>
       <c r="I671" t="inlineStr">
         <is>
-          <t>30-10-2025 05:04:39</t>
+          <t>03-11-2025 06:09:37</t>
         </is>
       </c>
       <c r="J671" t="inlineStr">
@@ -27677,7 +27677,7 @@
       </c>
       <c r="I673" t="inlineStr">
         <is>
-          <t>30-10-2025 05:06:26</t>
+          <t>03-11-2025 06:09:44</t>
         </is>
       </c>
       <c r="J673" t="inlineStr">
@@ -27757,7 +27757,7 @@
       </c>
       <c r="I675" t="inlineStr">
         <is>
-          <t>30-10-2025 05:08:12</t>
+          <t>03-11-2025 06:09:52</t>
         </is>
       </c>
       <c r="J675" t="inlineStr">
@@ -27837,7 +27837,7 @@
       </c>
       <c r="I677" t="inlineStr">
         <is>
-          <t>30-10-2025 05:10:03</t>
+          <t>03-11-2025 06:09:59</t>
         </is>
       </c>
       <c r="J677" t="inlineStr">
@@ -27917,7 +27917,7 @@
       </c>
       <c r="I679" t="inlineStr">
         <is>
-          <t>30-10-2025 05:11:51</t>
+          <t>03-11-2025 06:10:07</t>
         </is>
       </c>
       <c r="J679" t="inlineStr">
@@ -27997,7 +27997,7 @@
       </c>
       <c r="I681" t="inlineStr">
         <is>
-          <t>30-10-2025 05:13:39</t>
+          <t>03-11-2025 06:10:14</t>
         </is>
       </c>
       <c r="J681" t="inlineStr">
@@ -28117,7 +28117,7 @@
       </c>
       <c r="I684" t="inlineStr">
         <is>
-          <t>30-10-2025 05:18:27</t>
+          <t>03-11-2025 06:10:21</t>
         </is>
       </c>
       <c r="J684" t="inlineStr">
@@ -28197,7 +28197,7 @@
       </c>
       <c r="I686" t="inlineStr">
         <is>
-          <t>30-10-2025 05:20:14</t>
+          <t>03-11-2025 06:10:29</t>
         </is>
       </c>
       <c r="J686" t="inlineStr">
@@ -28277,7 +28277,7 @@
       </c>
       <c r="I688" t="inlineStr">
         <is>
-          <t>30-10-2025 05:22:00</t>
+          <t>03-11-2025 06:10:36</t>
         </is>
       </c>
       <c r="J688" t="inlineStr">
@@ -28597,7 +28597,7 @@
       </c>
       <c r="I696" t="inlineStr">
         <is>
-          <t>30-10-2025 05:43:04</t>
+          <t>03-11-2025 06:10:45</t>
         </is>
       </c>
       <c r="J696" t="inlineStr">
@@ -28677,7 +28677,7 @@
       </c>
       <c r="I698" t="inlineStr">
         <is>
-          <t>30-10-2025 05:44:51</t>
+          <t>03-11-2025 06:10:53</t>
         </is>
       </c>
       <c r="J698" t="inlineStr">
@@ -28757,7 +28757,7 @@
       </c>
       <c r="I700" t="inlineStr">
         <is>
-          <t>30-10-2025 05:46:38</t>
+          <t>03-11-2025 06:11:00</t>
         </is>
       </c>
       <c r="J700" t="inlineStr">
@@ -28877,7 +28877,7 @@
       </c>
       <c r="I703" t="inlineStr">
         <is>
-          <t>30-10-2025 05:51:55</t>
+          <t>03-11-2025 06:11:07</t>
         </is>
       </c>
       <c r="J703" t="inlineStr">
@@ -28957,7 +28957,7 @@
       </c>
       <c r="I705" t="inlineStr">
         <is>
-          <t>30-10-2025 05:53:42</t>
+          <t>03-11-2025 06:11:15</t>
         </is>
       </c>
       <c r="J705" t="inlineStr">
@@ -28995,6 +28995,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I706" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:11:23</t>
+        </is>
+      </c>
+      <c r="J706" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="707">
       <c r="A707" t="inlineStr">
@@ -29025,6 +29035,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I707" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:11:31</t>
+        </is>
+      </c>
+      <c r="J707" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="708">
       <c r="A708" t="inlineStr">
@@ -29055,6 +29075,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I708" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:11:38</t>
+        </is>
+      </c>
+      <c r="J708" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="709">
       <c r="A709" t="inlineStr">
@@ -29085,6 +29115,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I709" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:11:46</t>
+        </is>
+      </c>
+      <c r="J709" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="710">
       <c r="A710" t="inlineStr">
@@ -29115,6 +29155,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I710" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:11:53</t>
+        </is>
+      </c>
+      <c r="J710" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="711">
       <c r="A711" t="inlineStr">
@@ -29145,6 +29195,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I711" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:01</t>
+        </is>
+      </c>
+      <c r="J711" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="712">
       <c r="A712" t="inlineStr">
@@ -29175,6 +29235,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I712" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:08</t>
+        </is>
+      </c>
+      <c r="J712" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="713">
       <c r="A713" t="inlineStr">
@@ -29205,6 +29275,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I713" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:15</t>
+        </is>
+      </c>
+      <c r="J713" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="714">
       <c r="A714" t="inlineStr">
@@ -29235,6 +29315,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I714" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:23</t>
+        </is>
+      </c>
+      <c r="J714" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="715">
       <c r="A715" t="inlineStr">
@@ -29265,6 +29355,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I715" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:30</t>
+        </is>
+      </c>
+      <c r="J715" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="716">
       <c r="A716" t="inlineStr">
@@ -29295,6 +29395,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I716" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:37</t>
+        </is>
+      </c>
+      <c r="J716" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="717">
       <c r="A717" t="inlineStr">
@@ -29325,6 +29435,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I717" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:45</t>
+        </is>
+      </c>
+      <c r="J717" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="718">
       <c r="A718" t="inlineStr">
@@ -29355,6 +29475,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I718" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:52</t>
+        </is>
+      </c>
+      <c r="J718" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="719">
       <c r="A719" t="inlineStr">
@@ -29385,6 +29515,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I719" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:12:59</t>
+        </is>
+      </c>
+      <c r="J719" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="720">
       <c r="A720" t="inlineStr">
@@ -29415,6 +29555,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I720" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:07</t>
+        </is>
+      </c>
+      <c r="J720" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="721">
       <c r="A721" t="inlineStr">
@@ -29445,6 +29595,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I721" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:14</t>
+        </is>
+      </c>
+      <c r="J721" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="722">
       <c r="A722" t="inlineStr">
@@ -29475,6 +29635,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I722" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:22</t>
+        </is>
+      </c>
+      <c r="J722" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="723">
       <c r="A723" t="inlineStr">
@@ -29505,6 +29675,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I723" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:29</t>
+        </is>
+      </c>
+      <c r="J723" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="724">
       <c r="A724" t="inlineStr">
@@ -29535,6 +29715,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I724" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:37</t>
+        </is>
+      </c>
+      <c r="J724" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="725">
       <c r="A725" t="inlineStr">
@@ -29565,6 +29755,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I725" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:44</t>
+        </is>
+      </c>
+      <c r="J725" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="726">
       <c r="A726" t="inlineStr">
@@ -29595,6 +29795,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I726" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:52</t>
+        </is>
+      </c>
+      <c r="J726" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="727">
       <c r="A727" t="inlineStr">
@@ -29625,6 +29835,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I727" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:13:59</t>
+        </is>
+      </c>
+      <c r="J727" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="728">
       <c r="A728" t="inlineStr">
@@ -29655,6 +29875,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I728" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:06</t>
+        </is>
+      </c>
+      <c r="J728" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="729">
       <c r="A729" t="inlineStr">
@@ -29685,6 +29915,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I729" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:14</t>
+        </is>
+      </c>
+      <c r="J729" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="730">
       <c r="A730" t="inlineStr">
@@ -29715,6 +29955,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I730" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:21</t>
+        </is>
+      </c>
+      <c r="J730" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="731">
       <c r="A731" t="inlineStr">
@@ -29745,6 +29995,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I731" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:29</t>
+        </is>
+      </c>
+      <c r="J731" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="732">
       <c r="A732" t="inlineStr">
@@ -29775,6 +30035,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I732" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:36</t>
+        </is>
+      </c>
+      <c r="J732" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="733">
       <c r="A733" t="inlineStr">
@@ -29805,6 +30075,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I733" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:44</t>
+        </is>
+      </c>
+      <c r="J733" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="734">
       <c r="A734" t="inlineStr">
@@ -29835,6 +30115,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I734" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:51</t>
+        </is>
+      </c>
+      <c r="J734" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="735">
       <c r="A735" t="inlineStr">
@@ -29865,6 +30155,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I735" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:14:58</t>
+        </is>
+      </c>
+      <c r="J735" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="736">
       <c r="A736" t="inlineStr">
@@ -29895,6 +30195,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I736" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:06</t>
+        </is>
+      </c>
+      <c r="J736" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="737">
       <c r="A737" t="inlineStr">
@@ -29925,6 +30235,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I737" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:13</t>
+        </is>
+      </c>
+      <c r="J737" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="738">
       <c r="A738" t="inlineStr">
@@ -29955,6 +30275,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I738" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:20</t>
+        </is>
+      </c>
+      <c r="J738" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="739">
       <c r="A739" t="inlineStr">
@@ -29985,6 +30315,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I739" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:28</t>
+        </is>
+      </c>
+      <c r="J739" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="740">
       <c r="A740" t="inlineStr">
@@ -30015,6 +30355,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I740" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:35</t>
+        </is>
+      </c>
+      <c r="J740" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="741">
       <c r="A741" t="inlineStr">
@@ -30045,6 +30395,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I741" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:43</t>
+        </is>
+      </c>
+      <c r="J741" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="742">
       <c r="A742" t="inlineStr">
@@ -30075,6 +30435,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I742" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:50</t>
+        </is>
+      </c>
+      <c r="J742" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="743">
       <c r="A743" t="inlineStr">
@@ -30105,6 +30475,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I743" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:15:57</t>
+        </is>
+      </c>
+      <c r="J743" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="744">
       <c r="A744" t="inlineStr">
@@ -30135,6 +30515,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I744" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:04</t>
+        </is>
+      </c>
+      <c r="J744" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="745">
       <c r="A745" t="inlineStr">
@@ -30165,6 +30555,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I745" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:12</t>
+        </is>
+      </c>
+      <c r="J745" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="746">
       <c r="A746" t="inlineStr">
@@ -30195,6 +30595,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I746" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:19</t>
+        </is>
+      </c>
+      <c r="J746" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="747">
       <c r="A747" t="inlineStr">
@@ -30225,6 +30635,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I747" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:27</t>
+        </is>
+      </c>
+      <c r="J747" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="748">
       <c r="A748" t="inlineStr">
@@ -30255,6 +30675,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I748" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:35</t>
+        </is>
+      </c>
+      <c r="J748" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="749">
       <c r="A749" t="inlineStr">
@@ -30285,6 +30715,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I749" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:42</t>
+        </is>
+      </c>
+      <c r="J749" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="750">
       <c r="A750" t="inlineStr">
@@ -30315,6 +30755,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I750" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:49</t>
+        </is>
+      </c>
+      <c r="J750" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="751">
       <c r="A751" t="inlineStr">
@@ -30345,6 +30795,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I751" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:16:56</t>
+        </is>
+      </c>
+      <c r="J751" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="752">
       <c r="A752" t="inlineStr">
@@ -30375,6 +30835,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I752" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:04</t>
+        </is>
+      </c>
+      <c r="J752" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="753">
       <c r="A753" t="inlineStr">
@@ -30405,6 +30875,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I753" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:11</t>
+        </is>
+      </c>
+      <c r="J753" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="754">
       <c r="A754" t="inlineStr">
@@ -30435,6 +30915,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I754" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:19</t>
+        </is>
+      </c>
+      <c r="J754" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="755">
       <c r="A755" t="inlineStr">
@@ -30465,6 +30955,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I755" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:26</t>
+        </is>
+      </c>
+      <c r="J755" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="756">
       <c r="A756" t="inlineStr">
@@ -30495,6 +30995,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I756" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:34</t>
+        </is>
+      </c>
+      <c r="J756" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="757">
       <c r="A757" t="inlineStr">
@@ -30525,6 +31035,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I757" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:41</t>
+        </is>
+      </c>
+      <c r="J757" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="758">
       <c r="A758" t="inlineStr">
@@ -30555,6 +31075,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I758" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:48</t>
+        </is>
+      </c>
+      <c r="J758" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="759">
       <c r="A759" t="inlineStr">
@@ -30585,6 +31115,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I759" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:17:56</t>
+        </is>
+      </c>
+      <c r="J759" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="760">
       <c r="A760" t="inlineStr">
@@ -30615,6 +31155,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I760" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:03</t>
+        </is>
+      </c>
+      <c r="J760" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="761">
       <c r="A761" t="inlineStr">
@@ -30645,6 +31195,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I761" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:11</t>
+        </is>
+      </c>
+      <c r="J761" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="762">
       <c r="A762" t="inlineStr">
@@ -30675,6 +31235,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I762" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:18</t>
+        </is>
+      </c>
+      <c r="J762" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="763">
       <c r="A763" t="inlineStr">
@@ -30705,6 +31275,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I763" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:26</t>
+        </is>
+      </c>
+      <c r="J763" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="764">
       <c r="A764" t="inlineStr">
@@ -30735,6 +31315,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I764" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:33</t>
+        </is>
+      </c>
+      <c r="J764" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="765">
       <c r="A765" t="inlineStr">
@@ -30765,6 +31355,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I765" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:40</t>
+        </is>
+      </c>
+      <c r="J765" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="766">
       <c r="A766" t="inlineStr">
@@ -30795,6 +31395,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I766" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:48</t>
+        </is>
+      </c>
+      <c r="J766" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="767">
       <c r="A767" t="inlineStr">
@@ -30825,6 +31435,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I767" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:18:56</t>
+        </is>
+      </c>
+      <c r="J767" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="768">
       <c r="A768" t="inlineStr">
@@ -30855,6 +31475,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I768" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:03</t>
+        </is>
+      </c>
+      <c r="J768" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="769">
       <c r="A769" t="inlineStr">
@@ -30885,6 +31515,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I769" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:11</t>
+        </is>
+      </c>
+      <c r="J769" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="770">
       <c r="A770" t="inlineStr">
@@ -30915,6 +31555,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I770" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:18</t>
+        </is>
+      </c>
+      <c r="J770" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="771">
       <c r="A771" t="inlineStr">
@@ -30945,6 +31595,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I771" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:25</t>
+        </is>
+      </c>
+      <c r="J771" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="772">
       <c r="A772" t="inlineStr">
@@ -30975,6 +31635,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I772" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:33</t>
+        </is>
+      </c>
+      <c r="J772" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="773">
       <c r="A773" t="inlineStr">
@@ -31005,6 +31675,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I773" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:40</t>
+        </is>
+      </c>
+      <c r="J773" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="774">
       <c r="A774" t="inlineStr">
@@ -31035,6 +31715,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I774" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:47</t>
+        </is>
+      </c>
+      <c r="J774" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="775">
       <c r="A775" t="inlineStr">
@@ -31065,6 +31755,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I775" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:19:55</t>
+        </is>
+      </c>
+      <c r="J775" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="776">
       <c r="A776" t="inlineStr">
@@ -31095,6 +31795,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I776" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:03</t>
+        </is>
+      </c>
+      <c r="J776" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="777">
       <c r="A777" t="inlineStr">
@@ -31125,6 +31835,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I777" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:10</t>
+        </is>
+      </c>
+      <c r="J777" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="778">
       <c r="A778" t="inlineStr">
@@ -31155,6 +31875,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I778" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:17</t>
+        </is>
+      </c>
+      <c r="J778" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="779">
       <c r="A779" t="inlineStr">
@@ -31185,6 +31915,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I779" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:25</t>
+        </is>
+      </c>
+      <c r="J779" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="780">
       <c r="A780" t="inlineStr">
@@ -31215,6 +31955,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I780" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:32</t>
+        </is>
+      </c>
+      <c r="J780" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="781">
       <c r="A781" t="inlineStr">
@@ -31245,6 +31995,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I781" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:40</t>
+        </is>
+      </c>
+      <c r="J781" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="782">
       <c r="A782" t="inlineStr">
@@ -31275,6 +32035,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I782" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:47</t>
+        </is>
+      </c>
+      <c r="J782" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="783">
       <c r="A783" t="inlineStr">
@@ -31305,6 +32075,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I783" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:20:55</t>
+        </is>
+      </c>
+      <c r="J783" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="784">
       <c r="A784" t="inlineStr">
@@ -31335,6 +32115,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I784" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:02</t>
+        </is>
+      </c>
+      <c r="J784" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="785">
       <c r="A785" t="inlineStr">
@@ -31365,6 +32155,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I785" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:10</t>
+        </is>
+      </c>
+      <c r="J785" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="786">
       <c r="A786" t="inlineStr">
@@ -31395,6 +32195,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I786" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:17</t>
+        </is>
+      </c>
+      <c r="J786" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="787">
       <c r="A787" t="inlineStr">
@@ -31425,6 +32235,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I787" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:24</t>
+        </is>
+      </c>
+      <c r="J787" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="788">
       <c r="A788" t="inlineStr">
@@ -31455,6 +32275,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I788" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:32</t>
+        </is>
+      </c>
+      <c r="J788" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="789">
       <c r="A789" t="inlineStr">
@@ -31485,6 +32315,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I789" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:39</t>
+        </is>
+      </c>
+      <c r="J789" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="790">
       <c r="A790" t="inlineStr">
@@ -31515,6 +32355,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I790" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:47</t>
+        </is>
+      </c>
+      <c r="J790" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="791">
       <c r="A791" t="inlineStr">
@@ -31545,6 +32395,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I791" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:21:54</t>
+        </is>
+      </c>
+      <c r="J791" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="792">
       <c r="A792" t="inlineStr">
@@ -31575,6 +32435,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I792" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:02</t>
+        </is>
+      </c>
+      <c r="J792" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="793">
       <c r="A793" t="inlineStr">
@@ -31605,6 +32475,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I793" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:09</t>
+        </is>
+      </c>
+      <c r="J793" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="794">
       <c r="A794" t="inlineStr">
@@ -31635,6 +32515,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I794" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:16</t>
+        </is>
+      </c>
+      <c r="J794" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="795">
       <c r="A795" t="inlineStr">
@@ -31665,6 +32555,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I795" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:24</t>
+        </is>
+      </c>
+      <c r="J795" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="796">
       <c r="A796" t="inlineStr">
@@ -31695,6 +32595,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I796" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:31</t>
+        </is>
+      </c>
+      <c r="J796" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="797">
       <c r="A797" t="inlineStr">
@@ -31725,6 +32635,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I797" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:39</t>
+        </is>
+      </c>
+      <c r="J797" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="798">
       <c r="A798" t="inlineStr">
@@ -31755,6 +32675,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I798" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:46</t>
+        </is>
+      </c>
+      <c r="J798" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="799">
       <c r="A799" t="inlineStr">
@@ -31785,6 +32715,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I799" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:22:53</t>
+        </is>
+      </c>
+      <c r="J799" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="800">
       <c r="A800" t="inlineStr">
@@ -31815,6 +32755,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I800" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:01</t>
+        </is>
+      </c>
+      <c r="J800" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="801">
       <c r="A801" t="inlineStr">
@@ -31845,6 +32795,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I801" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:09</t>
+        </is>
+      </c>
+      <c r="J801" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="802">
       <c r="A802" t="inlineStr">
@@ -31875,6 +32835,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I802" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:16</t>
+        </is>
+      </c>
+      <c r="J802" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="803">
       <c r="A803" t="inlineStr">
@@ -31905,6 +32875,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I803" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:24</t>
+        </is>
+      </c>
+      <c r="J803" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="804">
       <c r="A804" t="inlineStr">
@@ -31935,6 +32915,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I804" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:31</t>
+        </is>
+      </c>
+      <c r="J804" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="805">
       <c r="A805" t="inlineStr">
@@ -31965,6 +32955,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I805" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:38</t>
+        </is>
+      </c>
+      <c r="J805" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="806">
       <c r="A806" t="inlineStr">
@@ -31995,6 +32995,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I806" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:46</t>
+        </is>
+      </c>
+      <c r="J806" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="807">
       <c r="A807" t="inlineStr">
@@ -32025,6 +33035,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I807" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:23:53</t>
+        </is>
+      </c>
+      <c r="J807" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="808">
       <c r="A808" t="inlineStr">
@@ -32055,6 +33075,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I808" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:01</t>
+        </is>
+      </c>
+      <c r="J808" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="809">
       <c r="A809" t="inlineStr">
@@ -32085,6 +33115,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I809" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:08</t>
+        </is>
+      </c>
+      <c r="J809" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="810">
       <c r="A810" t="inlineStr">
@@ -32115,6 +33155,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I810" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:15</t>
+        </is>
+      </c>
+      <c r="J810" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="811">
       <c r="A811" t="inlineStr">
@@ -32145,6 +33195,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I811" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:23</t>
+        </is>
+      </c>
+      <c r="J811" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="812">
       <c r="A812" t="inlineStr">
@@ -32175,6 +33235,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I812" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:30</t>
+        </is>
+      </c>
+      <c r="J812" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="813">
       <c r="A813" t="inlineStr">
@@ -32205,6 +33275,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I813" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:37</t>
+        </is>
+      </c>
+      <c r="J813" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="814">
       <c r="A814" t="inlineStr">
@@ -32235,6 +33315,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I814" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:45</t>
+        </is>
+      </c>
+      <c r="J814" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="815">
       <c r="A815" t="inlineStr">
@@ -32265,6 +33355,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I815" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:52</t>
+        </is>
+      </c>
+      <c r="J815" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="816">
       <c r="A816" t="inlineStr">
@@ -32295,6 +33395,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I816" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:24:59</t>
+        </is>
+      </c>
+      <c r="J816" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="817">
       <c r="A817" t="inlineStr">
@@ -32325,6 +33435,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I817" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:25:07</t>
+        </is>
+      </c>
+      <c r="J817" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="818">
       <c r="A818" t="inlineStr">
@@ -32355,6 +33475,16 @@
           <t>Pendiente</t>
         </is>
       </c>
+      <c r="I818" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:25:14</t>
+        </is>
+      </c>
+      <c r="J818" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
+        </is>
+      </c>
     </row>
     <row r="819">
       <c r="A819" t="inlineStr">
@@ -32383,6 +33513,16 @@
       <c r="H819" t="inlineStr">
         <is>
           <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="I819" t="inlineStr">
+        <is>
+          <t>03-11-2025 06:25:22</t>
+        </is>
+      </c>
+      <c r="J819" t="inlineStr">
+        <is>
+          <t>Ocurrio un error al abrir Workmanager. Revisar archivo de logs.</t>
         </is>
       </c>
     </row>

</xml_diff>